<commit_message>
trivial changes in file great
</commit_message>
<xml_diff>
--- a/codes_and_dfs/SemCor_interactive_df_great.xlsx
+++ b/codes_and_dfs/SemCor_interactive_df_great.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rezas\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rezas\OneDrive\Desktop\ContextLens\codes_and_dfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EA6F80-83C8-4BAC-A9C4-AEF6657C664D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104343B4-FF3C-4550-AFA3-E7394A743240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-825" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -986,10 +999,13 @@
   <dimension ref="A1:Z175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1162,7 +1178,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1242,7 +1258,7 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1322,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1402,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1482,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1882,7 +1898,7 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -2042,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -2122,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -2282,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -2362,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2442,7 +2458,7 @@
         <v>4</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -2602,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -2682,7 +2698,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -2762,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2842,7 +2858,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2922,7 +2938,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -3002,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -3402,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -3482,7 +3498,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -3642,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -3722,7 +3738,7 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -3802,7 +3818,7 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -3882,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -3962,7 +3978,7 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -4042,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -4122,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -4202,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -4282,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -4442,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -4522,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -4602,7 +4618,7 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -4682,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -4762,7 +4778,7 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -4922,7 +4938,7 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -5002,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -5082,7 +5098,7 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -5162,7 +5178,7 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -5242,7 +5258,7 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -5322,7 +5338,7 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -5402,7 +5418,7 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -5482,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -5562,7 +5578,7 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
         <v>2</v>
@@ -5642,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>3</v>
@@ -5722,7 +5738,7 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -5802,7 +5818,7 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -5882,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
         <v>3</v>
@@ -5962,7 +5978,7 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -6042,7 +6058,7 @@
         <v>1</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -6122,7 +6138,7 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -6202,7 +6218,7 @@
         <v>1</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -6362,7 +6378,7 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -6442,7 +6458,7 @@
         <v>1</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -6522,7 +6538,7 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -6602,7 +6618,7 @@
         <v>1</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -6682,7 +6698,7 @@
         <v>1</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -6842,7 +6858,7 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -6922,7 +6938,7 @@
         <v>1</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -7002,7 +7018,7 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -7082,7 +7098,7 @@
         <v>1</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77">
         <v>2</v>
@@ -7162,7 +7178,7 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -7242,7 +7258,7 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79">
         <v>3</v>
@@ -7322,7 +7338,7 @@
         <v>0</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -7482,7 +7498,7 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -7882,7 +7898,7 @@
         <v>3</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -8042,7 +8058,7 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -8122,7 +8138,7 @@
         <v>1</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -8202,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -8282,7 +8298,7 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -8362,7 +8378,7 @@
         <v>3</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -8522,7 +8538,7 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -8602,7 +8618,7 @@
         <v>1</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E96">
         <v>3</v>
@@ -8682,7 +8698,7 @@
         <v>1</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -8842,7 +8858,7 @@
         <v>1</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -8922,7 +8938,7 @@
         <v>1</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -9002,7 +9018,7 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -9082,7 +9098,7 @@
         <v>1</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -9162,7 +9178,7 @@
         <v>1</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -9242,7 +9258,7 @@
         <v>1</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -9322,7 +9338,7 @@
         <v>1</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E105">
         <v>0</v>
@@ -9402,7 +9418,7 @@
         <v>1</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -9482,7 +9498,7 @@
         <v>0</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -9562,7 +9578,7 @@
         <v>1</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -9642,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -9722,7 +9738,7 @@
         <v>1</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -9802,7 +9818,7 @@
         <v>1</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -9882,7 +9898,7 @@
         <v>1</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E112">
         <v>3</v>
@@ -9962,7 +9978,7 @@
         <v>1</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E113">
         <v>3</v>
@@ -10042,7 +10058,7 @@
         <v>1</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E114">
         <v>0</v>
@@ -10122,7 +10138,7 @@
         <v>1</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E115">
         <v>1</v>
@@ -10202,7 +10218,7 @@
         <v>1</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E116">
         <v>3</v>
@@ -10362,7 +10378,7 @@
         <v>0</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -10442,7 +10458,7 @@
         <v>1</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -10522,7 +10538,7 @@
         <v>0</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -10842,7 +10858,7 @@
         <v>0</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -10922,7 +10938,7 @@
         <v>0</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E125">
         <v>3</v>
@@ -11002,7 +11018,7 @@
         <v>0</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E126">
         <v>0</v>
@@ -11082,7 +11098,7 @@
         <v>0</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E127">
         <v>3</v>
@@ -11162,7 +11178,7 @@
         <v>0</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128">
         <v>3</v>
@@ -11242,7 +11258,7 @@
         <v>0</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129">
         <v>2</v>
@@ -11322,7 +11338,7 @@
         <v>0</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130">
         <v>0</v>
@@ -11402,7 +11418,7 @@
         <v>0</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131">
         <v>3</v>
@@ -11722,7 +11738,7 @@
         <v>0</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E135">
         <v>0</v>
@@ -11962,7 +11978,7 @@
         <v>1</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E138">
         <v>0</v>
@@ -12122,7 +12138,7 @@
         <v>2</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -12202,7 +12218,7 @@
         <v>0</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E141">
         <v>0</v>
@@ -12442,7 +12458,7 @@
         <v>0</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -12522,7 +12538,7 @@
         <v>1</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -12682,7 +12698,7 @@
         <v>1</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E147">
         <v>3</v>
@@ -12762,7 +12778,7 @@
         <v>1</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E148">
         <v>0</v>
@@ -12842,7 +12858,7 @@
         <v>0</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149">
         <v>0</v>
@@ -12922,7 +12938,7 @@
         <v>1</v>
       </c>
       <c r="D150">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E150">
         <v>3</v>
@@ -13002,7 +13018,7 @@
         <v>0</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E151">
         <v>0</v>
@@ -13082,7 +13098,7 @@
         <v>1</v>
       </c>
       <c r="D152">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E152">
         <v>3</v>
@@ -13162,7 +13178,7 @@
         <v>3</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E153">
         <v>0</v>
@@ -13242,7 +13258,7 @@
         <v>0</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E154">
         <v>0</v>
@@ -13322,7 +13338,7 @@
         <v>1</v>
       </c>
       <c r="D155">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E155">
         <v>3</v>
@@ -13402,7 +13418,7 @@
         <v>0</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E156">
         <v>0</v>
@@ -13482,7 +13498,7 @@
         <v>0</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E157">
         <v>0</v>
@@ -13882,7 +13898,7 @@
         <v>1</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E162">
         <v>3</v>
@@ -13962,7 +13978,7 @@
         <v>1</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E163">
         <v>0</v>
@@ -14042,7 +14058,7 @@
         <v>1</v>
       </c>
       <c r="D164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E164">
         <v>3</v>
@@ -14122,7 +14138,7 @@
         <v>1</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E165">
         <v>1</v>
@@ -14202,7 +14218,7 @@
         <v>0</v>
       </c>
       <c r="D166">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E166">
         <v>0</v>
@@ -14362,7 +14378,7 @@
         <v>1</v>
       </c>
       <c r="D168">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -14442,7 +14458,7 @@
         <v>4</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E169">
         <v>2</v>
@@ -14602,7 +14618,7 @@
         <v>0</v>
       </c>
       <c r="D171">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E171">
         <v>0</v>
@@ -14842,7 +14858,7 @@
         <v>0</v>
       </c>
       <c r="D174">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E174">
         <v>1</v>

</xml_diff>